<commit_message>
Update to 2025 MLLB Constants
</commit_message>
<xml_diff>
--- a/baseballStatistics/datasets/jimbo datasets/2025 MLB Constants.xlsx
+++ b/baseballStatistics/datasets/jimbo datasets/2025 MLB Constants.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="105">
   <si>
     <t>Season</t>
   </si>
@@ -63,12 +63,21 @@
     <t>NL wRC</t>
   </si>
   <si>
+    <t>AL PA</t>
+  </si>
+  <si>
+    <t>NL PA</t>
+  </si>
+  <si>
     <t>Team</t>
   </si>
   <si>
     <t>Abbreviation</t>
   </si>
   <si>
+    <t>League</t>
+  </si>
+  <si>
     <t>Basic (5yr)</t>
   </si>
   <si>
@@ -117,6 +126,9 @@
     <t>LAA</t>
   </si>
   <si>
+    <t>AL</t>
+  </si>
+  <si>
     <t>Orioles</t>
   </si>
   <si>
@@ -199,6 +211,9 @@
   </si>
   <si>
     <t>AZ</t>
+  </si>
+  <si>
+    <t>NL</t>
   </si>
   <si>
     <t>Braves</t>
@@ -639,8 +654,12 @@
       <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
       <c r="U1" s="3"/>
@@ -696,6 +715,12 @@
       </c>
       <c r="P2" s="4">
         <v>10865.0</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>91255.0</v>
+      </c>
+      <c r="R2" s="4">
+        <v>91663.0</v>
       </c>
     </row>
     <row r="3">
@@ -7494,52 +7519,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="2">
@@ -7547,13 +7575,13 @@
         <v>2025.0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="4">
-        <v>101.0</v>
+        <v>36</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="E2" s="4">
         <v>101.0</v>
@@ -7562,22 +7590,22 @@
         <v>101.0</v>
       </c>
       <c r="G2" s="4">
+        <v>101.0</v>
+      </c>
+      <c r="H2" s="4">
         <v>100.0</v>
       </c>
-      <c r="H2" s="4">
+      <c r="I2" s="4">
         <v>97.0</v>
       </c>
-      <c r="I2" s="4">
+      <c r="J2" s="4">
         <v>101.0</v>
       </c>
-      <c r="J2" s="4">
+      <c r="K2" s="4">
         <v>105.0</v>
       </c>
-      <c r="K2" s="4">
+      <c r="L2" s="4">
         <v>102.0</v>
-      </c>
-      <c r="L2" s="4">
-        <v>100.0</v>
       </c>
       <c r="M2" s="4">
         <v>100.0</v>
@@ -7586,12 +7614,15 @@
         <v>100.0</v>
       </c>
       <c r="O2" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="P2" s="4">
         <v>102.0</v>
       </c>
-      <c r="P2" s="4">
+      <c r="Q2" s="4">
         <v>92.0</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="R2" s="4">
         <v>101.0</v>
       </c>
     </row>
@@ -7600,51 +7631,54 @@
         <v>2025.0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="4">
+        <v>39</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="4">
         <v>99.0</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="4">
         <v>98.0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>103.0</v>
       </c>
       <c r="G3" s="4">
         <v>103.0</v>
       </c>
       <c r="H3" s="4">
+        <v>103.0</v>
+      </c>
+      <c r="I3" s="4">
         <v>96.0</v>
       </c>
-      <c r="I3" s="4">
+      <c r="J3" s="4">
         <v>101.0</v>
-      </c>
-      <c r="J3" s="4">
-        <v>99.0</v>
       </c>
       <c r="K3" s="4">
         <v>99.0</v>
       </c>
       <c r="L3" s="4">
+        <v>99.0</v>
+      </c>
+      <c r="M3" s="4">
         <v>97.0</v>
-      </c>
-      <c r="M3" s="4">
-        <v>100.0</v>
       </c>
       <c r="N3" s="4">
         <v>100.0</v>
       </c>
       <c r="O3" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="P3" s="4">
         <v>103.0</v>
       </c>
-      <c r="P3" s="4">
+      <c r="Q3" s="4">
         <v>98.0</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="R3" s="4">
         <v>99.0</v>
       </c>
     </row>
@@ -7653,51 +7687,54 @@
         <v>2025.0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="4">
         <v>104.0</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="4">
         <v>102.0</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="4">
         <v>100.0</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="4">
         <v>104.0</v>
       </c>
-      <c r="H4" s="4">
+      <c r="I4" s="4">
         <v>109.0</v>
       </c>
-      <c r="I4" s="4">
+      <c r="J4" s="4">
         <v>115.0</v>
-      </c>
-      <c r="J4" s="4">
-        <v>98.0</v>
       </c>
       <c r="K4" s="4">
         <v>98.0</v>
       </c>
       <c r="L4" s="4">
+        <v>98.0</v>
+      </c>
+      <c r="M4" s="4">
         <v>101.0</v>
       </c>
-      <c r="M4" s="4">
+      <c r="N4" s="4">
         <v>103.0</v>
       </c>
-      <c r="N4" s="4">
+      <c r="O4" s="4">
         <v>98.0</v>
       </c>
-      <c r="O4" s="4">
+      <c r="P4" s="4">
         <v>99.0</v>
       </c>
-      <c r="P4" s="4">
+      <c r="Q4" s="4">
         <v>101.0</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="R4" s="4">
         <v>100.0</v>
       </c>
     </row>
@@ -7706,51 +7743,54 @@
         <v>2025.0</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="4">
+        <v>43</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="4">
         <v>100.0</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="4">
         <v>98.0</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="4">
         <v>99.0</v>
       </c>
-      <c r="G5" s="4">
+      <c r="H5" s="4">
         <v>100.0</v>
       </c>
-      <c r="H5" s="4">
+      <c r="I5" s="4">
         <v>96.0</v>
       </c>
-      <c r="I5" s="4">
+      <c r="J5" s="4">
         <v>87.0</v>
       </c>
-      <c r="J5" s="4">
+      <c r="K5" s="4">
         <v>105.0</v>
       </c>
-      <c r="K5" s="4">
+      <c r="L5" s="4">
         <v>99.0</v>
       </c>
-      <c r="L5" s="4">
+      <c r="M5" s="4">
         <v>101.0</v>
       </c>
-      <c r="M5" s="4">
+      <c r="N5" s="4">
         <v>99.0</v>
       </c>
-      <c r="N5" s="4">
+      <c r="O5" s="4">
         <v>105.0</v>
       </c>
-      <c r="O5" s="4">
+      <c r="P5" s="4">
         <v>98.0</v>
       </c>
-      <c r="P5" s="4">
+      <c r="Q5" s="4">
         <v>104.0</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="R5" s="4">
         <v>103.0</v>
       </c>
     </row>
@@ -7759,16 +7799,16 @@
         <v>2025.0</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="4">
+        <v>45</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="4">
         <v>99.0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>100.0</v>
       </c>
       <c r="F6" s="4">
         <v>100.0</v>
@@ -7780,30 +7820,33 @@
         <v>100.0</v>
       </c>
       <c r="I6" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="J6" s="4">
         <v>87.0</v>
       </c>
-      <c r="J6" s="4">
+      <c r="K6" s="4">
         <v>98.0</v>
-      </c>
-      <c r="K6" s="4">
-        <v>101.0</v>
       </c>
       <c r="L6" s="4">
         <v>101.0</v>
       </c>
       <c r="M6" s="4">
+        <v>101.0</v>
+      </c>
+      <c r="N6" s="4">
         <v>100.0</v>
       </c>
-      <c r="N6" s="4">
+      <c r="O6" s="4">
         <v>96.0</v>
       </c>
-      <c r="O6" s="4">
+      <c r="P6" s="4">
         <v>98.0</v>
       </c>
-      <c r="P6" s="4">
+      <c r="Q6" s="4">
         <v>96.0</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="R6" s="4">
         <v>99.0</v>
       </c>
     </row>
@@ -7812,51 +7855,54 @@
         <v>2025.0</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="4">
+        <v>47</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="4">
         <v>100.0</v>
       </c>
-      <c r="E7" s="4">
+      <c r="F7" s="4">
         <v>103.0</v>
       </c>
-      <c r="F7" s="4">
+      <c r="G7" s="4">
         <v>104.0</v>
-      </c>
-      <c r="G7" s="4">
-        <v>100.0</v>
       </c>
       <c r="H7" s="4">
         <v>100.0</v>
       </c>
       <c r="I7" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="J7" s="4">
         <v>118.0</v>
       </c>
-      <c r="J7" s="4">
+      <c r="K7" s="4">
         <v>96.0</v>
       </c>
-      <c r="K7" s="4">
+      <c r="L7" s="4">
         <v>98.0</v>
       </c>
-      <c r="L7" s="4">
+      <c r="M7" s="4">
         <v>102.0</v>
       </c>
-      <c r="M7" s="4">
+      <c r="N7" s="4">
         <v>99.0</v>
       </c>
-      <c r="N7" s="4">
+      <c r="O7" s="4">
         <v>102.0</v>
       </c>
-      <c r="O7" s="4">
+      <c r="P7" s="4">
         <v>101.0</v>
       </c>
-      <c r="P7" s="4">
+      <c r="Q7" s="4">
         <v>108.0</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="R7" s="4">
         <v>100.0</v>
       </c>
     </row>
@@ -7865,51 +7911,54 @@
         <v>2025.0</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="4">
-        <v>103.0</v>
+        <v>49</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="E8" s="4">
         <v>103.0</v>
       </c>
       <c r="F8" s="4">
+        <v>103.0</v>
+      </c>
+      <c r="G8" s="4">
         <v>95.0</v>
       </c>
-      <c r="G8" s="4">
+      <c r="H8" s="4">
         <v>103.0</v>
       </c>
-      <c r="H8" s="4">
+      <c r="I8" s="4">
         <v>108.0</v>
       </c>
-      <c r="I8" s="4">
+      <c r="J8" s="4">
         <v>123.0</v>
       </c>
-      <c r="J8" s="4">
+      <c r="K8" s="4">
         <v>95.0</v>
       </c>
-      <c r="K8" s="4">
+      <c r="L8" s="4">
         <v>97.0</v>
       </c>
-      <c r="L8" s="4">
+      <c r="M8" s="4">
         <v>101.0</v>
       </c>
-      <c r="M8" s="4">
+      <c r="N8" s="4">
         <v>103.0</v>
       </c>
-      <c r="N8" s="4">
+      <c r="O8" s="4">
         <v>101.0</v>
       </c>
-      <c r="O8" s="4">
+      <c r="P8" s="4">
         <v>105.0</v>
       </c>
-      <c r="P8" s="4">
+      <c r="Q8" s="4">
         <v>96.0</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="R8" s="4">
         <v>100.0</v>
       </c>
     </row>
@@ -7918,51 +7967,54 @@
         <v>2025.0</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="4">
+        <v>51</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="4">
         <v>101.0</v>
       </c>
-      <c r="E9" s="4">
+      <c r="F9" s="4">
         <v>103.0</v>
       </c>
-      <c r="F9" s="4">
+      <c r="G9" s="4">
         <v>106.0</v>
       </c>
-      <c r="G9" s="4">
+      <c r="H9" s="4">
         <v>101.0</v>
       </c>
-      <c r="H9" s="4">
+      <c r="I9" s="4">
         <v>105.0</v>
       </c>
-      <c r="I9" s="4">
+      <c r="J9" s="4">
         <v>93.0</v>
       </c>
-      <c r="J9" s="4">
+      <c r="K9" s="4">
         <v>99.0</v>
       </c>
-      <c r="K9" s="4">
+      <c r="L9" s="4">
         <v>100.0</v>
       </c>
-      <c r="L9" s="4">
+      <c r="M9" s="4">
         <v>103.0</v>
       </c>
-      <c r="M9" s="4">
+      <c r="N9" s="4">
         <v>99.0</v>
       </c>
-      <c r="N9" s="4">
+      <c r="O9" s="4">
         <v>101.0</v>
       </c>
-      <c r="O9" s="4">
+      <c r="P9" s="4">
         <v>97.0</v>
       </c>
-      <c r="P9" s="4">
+      <c r="Q9" s="4">
         <v>103.0</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="R9" s="4">
         <v>100.0</v>
       </c>
     </row>
@@ -7971,51 +8023,54 @@
         <v>2025.0</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="4">
-        <v>99.0</v>
+        <v>53</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="E10" s="4">
         <v>99.0</v>
       </c>
       <c r="F10" s="4">
+        <v>99.0</v>
+      </c>
+      <c r="G10" s="4">
         <v>96.0</v>
       </c>
-      <c r="G10" s="4">
+      <c r="H10" s="4">
         <v>97.0</v>
       </c>
-      <c r="H10" s="4">
+      <c r="I10" s="4">
         <v>95.0</v>
       </c>
-      <c r="I10" s="4">
+      <c r="J10" s="4">
         <v>85.0</v>
       </c>
-      <c r="J10" s="4">
+      <c r="K10" s="4">
         <v>104.0</v>
       </c>
-      <c r="K10" s="4">
+      <c r="L10" s="4">
         <v>100.0</v>
       </c>
-      <c r="L10" s="4">
+      <c r="M10" s="4">
         <v>101.0</v>
       </c>
-      <c r="M10" s="4">
+      <c r="N10" s="4">
         <v>98.0</v>
       </c>
-      <c r="N10" s="4">
+      <c r="O10" s="4">
         <v>105.0</v>
       </c>
-      <c r="O10" s="4">
+      <c r="P10" s="4">
         <v>97.0</v>
       </c>
-      <c r="P10" s="4">
+      <c r="Q10" s="4">
         <v>102.0</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="R10" s="4">
         <v>102.0</v>
       </c>
     </row>
@@ -8024,51 +8079,54 @@
         <v>2025.0</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="4">
+        <v>55</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="4">
         <v>103.0</v>
-      </c>
-      <c r="E11" s="4">
-        <v>105.0</v>
       </c>
       <c r="F11" s="4">
         <v>105.0</v>
       </c>
       <c r="G11" s="4">
+        <v>105.0</v>
+      </c>
+      <c r="H11" s="4">
         <v>102.0</v>
       </c>
-      <c r="H11" s="4">
+      <c r="I11" s="4">
         <v>107.0</v>
       </c>
-      <c r="I11" s="4">
+      <c r="J11" s="4">
         <v>96.0</v>
       </c>
-      <c r="J11" s="4">
+      <c r="K11" s="4">
         <v>103.0</v>
       </c>
-      <c r="K11" s="4">
+      <c r="L11" s="4">
         <v>101.0</v>
       </c>
-      <c r="L11" s="4">
+      <c r="M11" s="4">
         <v>103.0</v>
-      </c>
-      <c r="M11" s="4">
-        <v>100.0</v>
       </c>
       <c r="N11" s="4">
         <v>100.0</v>
       </c>
       <c r="O11" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="P11" s="4">
         <v>105.0</v>
       </c>
-      <c r="P11" s="4">
+      <c r="Q11" s="4">
         <v>112.0</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="R11" s="4">
         <v>102.0</v>
       </c>
     </row>
@@ -8077,51 +8135,54 @@
         <v>2025.0</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="4">
+        <v>57</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="4">
         <v>94.0</v>
       </c>
-      <c r="E12" s="4">
+      <c r="F12" s="4">
         <v>92.0</v>
       </c>
-      <c r="F12" s="4">
+      <c r="G12" s="4">
         <v>91.0</v>
       </c>
-      <c r="G12" s="4">
+      <c r="H12" s="4">
         <v>95.0</v>
       </c>
-      <c r="H12" s="4">
+      <c r="I12" s="4">
         <v>93.0</v>
       </c>
-      <c r="I12" s="4">
+      <c r="J12" s="4">
         <v>79.0</v>
       </c>
-      <c r="J12" s="4">
+      <c r="K12" s="4">
         <v>96.0</v>
       </c>
-      <c r="K12" s="4">
+      <c r="L12" s="4">
         <v>104.0</v>
-      </c>
-      <c r="L12" s="4">
-        <v>97.0</v>
       </c>
       <c r="M12" s="4">
         <v>97.0</v>
       </c>
       <c r="N12" s="4">
+        <v>97.0</v>
+      </c>
+      <c r="O12" s="4">
         <v>99.0</v>
       </c>
-      <c r="O12" s="4">
+      <c r="P12" s="4">
         <v>96.0</v>
       </c>
-      <c r="P12" s="4">
+      <c r="Q12" s="4">
         <v>105.0</v>
       </c>
-      <c r="Q12" s="4">
+      <c r="R12" s="4">
         <v>96.0</v>
       </c>
     </row>
@@ -8130,51 +8191,54 @@
         <v>2025.0</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="4">
+        <v>59</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="4">
         <v>101.0</v>
-      </c>
-      <c r="E13" s="4">
-        <v>102.0</v>
       </c>
       <c r="F13" s="4">
         <v>102.0</v>
       </c>
       <c r="G13" s="4">
+        <v>102.0</v>
+      </c>
+      <c r="H13" s="4">
         <v>103.0</v>
       </c>
-      <c r="H13" s="4">
+      <c r="I13" s="4">
         <v>96.0</v>
       </c>
-      <c r="I13" s="4">
+      <c r="J13" s="4">
         <v>88.0</v>
       </c>
-      <c r="J13" s="4">
+      <c r="K13" s="4">
         <v>104.0</v>
-      </c>
-      <c r="K13" s="4">
-        <v>100.0</v>
       </c>
       <c r="L13" s="4">
         <v>100.0</v>
       </c>
       <c r="M13" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="N13" s="4">
         <v>102.0</v>
       </c>
-      <c r="N13" s="4">
+      <c r="O13" s="4">
         <v>97.0</v>
       </c>
-      <c r="O13" s="4">
+      <c r="P13" s="4">
         <v>102.0</v>
       </c>
-      <c r="P13" s="4">
+      <c r="Q13" s="4">
         <v>89.0</v>
       </c>
-      <c r="Q13" s="4">
+      <c r="R13" s="4">
         <v>102.0</v>
       </c>
     </row>
@@ -8183,51 +8247,54 @@
         <v>2025.0</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="4">
+        <v>61</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="4">
         <v>99.0</v>
       </c>
-      <c r="E14" s="4">
+      <c r="F14" s="4">
         <v>97.0</v>
       </c>
-      <c r="F14" s="4">
+      <c r="G14" s="4">
         <v>91.0</v>
       </c>
-      <c r="G14" s="4">
+      <c r="H14" s="4">
         <v>98.0</v>
       </c>
-      <c r="H14" s="4">
+      <c r="I14" s="4">
         <v>100.0</v>
       </c>
-      <c r="I14" s="4">
+      <c r="J14" s="4">
         <v>93.0</v>
       </c>
-      <c r="J14" s="4">
+      <c r="K14" s="4">
         <v>102.0</v>
       </c>
-      <c r="K14" s="4">
+      <c r="L14" s="4">
         <v>101.0</v>
       </c>
-      <c r="L14" s="4">
+      <c r="M14" s="4">
         <v>100.0</v>
       </c>
-      <c r="M14" s="4">
+      <c r="N14" s="4">
         <v>99.0</v>
       </c>
-      <c r="N14" s="4">
+      <c r="O14" s="4">
         <v>102.0</v>
       </c>
-      <c r="O14" s="4">
+      <c r="P14" s="4">
         <v>100.0</v>
       </c>
-      <c r="P14" s="4">
+      <c r="Q14" s="4">
         <v>97.0</v>
       </c>
-      <c r="Q14" s="4">
+      <c r="R14" s="4">
         <v>101.0</v>
       </c>
     </row>
@@ -8236,51 +8303,54 @@
         <v>2025.0</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="4">
+        <v>63</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="4">
         <v>99.0</v>
       </c>
-      <c r="E15" s="4">
+      <c r="F15" s="4">
         <v>100.0</v>
       </c>
-      <c r="F15" s="4">
+      <c r="G15" s="4">
         <v>101.0</v>
       </c>
-      <c r="G15" s="4">
+      <c r="H15" s="4">
         <v>98.0</v>
       </c>
-      <c r="H15" s="4">
+      <c r="I15" s="4">
         <v>102.0</v>
       </c>
-      <c r="I15" s="4">
+      <c r="J15" s="4">
         <v>90.0</v>
       </c>
-      <c r="J15" s="4">
+      <c r="K15" s="4">
         <v>103.0</v>
       </c>
-      <c r="K15" s="4">
+      <c r="L15" s="4">
         <v>100.0</v>
       </c>
-      <c r="L15" s="4">
+      <c r="M15" s="4">
         <v>99.0</v>
-      </c>
-      <c r="M15" s="4">
-        <v>100.0</v>
       </c>
       <c r="N15" s="4">
         <v>100.0</v>
       </c>
       <c r="O15" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="P15" s="4">
         <v>101.0</v>
       </c>
-      <c r="P15" s="4">
+      <c r="Q15" s="4">
         <v>100.0</v>
       </c>
-      <c r="Q15" s="4">
+      <c r="R15" s="4">
         <v>101.0</v>
       </c>
     </row>
@@ -8289,51 +8359,54 @@
         <v>2025.0</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="4">
+        <v>65</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="4">
         <v>101.0</v>
-      </c>
-      <c r="E16" s="4">
-        <v>100.0</v>
       </c>
       <c r="F16" s="4">
         <v>100.0</v>
       </c>
       <c r="G16" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="H16" s="4">
         <v>103.0</v>
       </c>
-      <c r="H16" s="4">
+      <c r="I16" s="4">
         <v>105.0</v>
       </c>
-      <c r="I16" s="4">
+      <c r="J16" s="4">
         <v>120.0</v>
       </c>
-      <c r="J16" s="4">
+      <c r="K16" s="4">
         <v>91.0</v>
-      </c>
-      <c r="K16" s="4">
-        <v>99.0</v>
       </c>
       <c r="L16" s="4">
         <v>99.0</v>
       </c>
       <c r="M16" s="4">
+        <v>99.0</v>
+      </c>
+      <c r="N16" s="4">
         <v>103.0</v>
       </c>
-      <c r="N16" s="4">
+      <c r="O16" s="4">
         <v>98.0</v>
       </c>
-      <c r="O16" s="4">
+      <c r="P16" s="4">
         <v>105.0</v>
       </c>
-      <c r="P16" s="4">
+      <c r="Q16" s="4">
         <v>97.0</v>
       </c>
-      <c r="Q16" s="4">
+      <c r="R16" s="4">
         <v>97.0</v>
       </c>
     </row>
@@ -8342,51 +8415,54 @@
         <v>2025.0</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" s="4">
-        <v>100.0</v>
+        <v>68</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="E17" s="4">
         <v>100.0</v>
       </c>
       <c r="F17" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="G17" s="4">
         <v>99.0</v>
       </c>
-      <c r="G17" s="4">
+      <c r="H17" s="4">
         <v>101.0</v>
       </c>
-      <c r="H17" s="4">
+      <c r="I17" s="4">
         <v>99.0</v>
       </c>
-      <c r="I17" s="4">
+      <c r="J17" s="4">
         <v>100.0</v>
       </c>
-      <c r="J17" s="4">
+      <c r="K17" s="4">
         <v>99.0</v>
       </c>
-      <c r="K17" s="4">
+      <c r="L17" s="4">
         <v>102.0</v>
       </c>
-      <c r="L17" s="4">
+      <c r="M17" s="4">
         <v>99.0</v>
       </c>
-      <c r="M17" s="4">
+      <c r="N17" s="4">
         <v>101.0</v>
       </c>
-      <c r="N17" s="4">
+      <c r="O17" s="4">
         <v>98.0</v>
       </c>
-      <c r="O17" s="4">
+      <c r="P17" s="4">
         <v>101.0</v>
       </c>
-      <c r="P17" s="4">
+      <c r="Q17" s="4">
         <v>94.0</v>
       </c>
-      <c r="Q17" s="4">
+      <c r="R17" s="4">
         <v>98.0</v>
       </c>
     </row>
@@ -8395,51 +8471,54 @@
         <v>2025.0</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="4">
+        <v>70</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="4">
         <v>98.0</v>
       </c>
-      <c r="E18" s="4">
+      <c r="F18" s="4">
         <v>96.0</v>
       </c>
-      <c r="F18" s="4">
+      <c r="G18" s="4">
         <v>99.0</v>
       </c>
-      <c r="G18" s="4">
+      <c r="H18" s="4">
         <v>100.0</v>
       </c>
-      <c r="H18" s="4">
+      <c r="I18" s="4">
         <v>94.0</v>
       </c>
-      <c r="I18" s="4">
+      <c r="J18" s="4">
         <v>109.0</v>
       </c>
-      <c r="J18" s="4">
+      <c r="K18" s="4">
         <v>98.0</v>
       </c>
-      <c r="K18" s="4">
+      <c r="L18" s="4">
         <v>101.0</v>
       </c>
-      <c r="L18" s="4">
+      <c r="M18" s="4">
         <v>99.0</v>
       </c>
-      <c r="M18" s="4">
+      <c r="N18" s="4">
         <v>100.0</v>
       </c>
-      <c r="N18" s="4">
+      <c r="O18" s="4">
         <v>97.0</v>
-      </c>
-      <c r="O18" s="4">
-        <v>100.0</v>
       </c>
       <c r="P18" s="4">
         <v>100.0</v>
       </c>
       <c r="Q18" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="R18" s="4">
         <v>98.0</v>
       </c>
     </row>
@@ -8448,51 +8527,54 @@
         <v>2025.0</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="4">
+      <c r="E19" s="4">
         <v>105.0</v>
       </c>
-      <c r="E19" s="4">
+      <c r="F19" s="4">
         <v>102.0</v>
       </c>
-      <c r="F19" s="4">
+      <c r="G19" s="4">
         <v>100.0</v>
-      </c>
-      <c r="G19" s="4">
-        <v>101.0</v>
       </c>
       <c r="H19" s="4">
         <v>101.0</v>
       </c>
       <c r="I19" s="4">
+        <v>101.0</v>
+      </c>
+      <c r="J19" s="4">
         <v>84.0</v>
       </c>
-      <c r="J19" s="4">
+      <c r="K19" s="4">
         <v>114.0</v>
       </c>
-      <c r="K19" s="4">
+      <c r="L19" s="4">
         <v>101.0</v>
       </c>
-      <c r="L19" s="4">
+      <c r="M19" s="4">
         <v>102.0</v>
       </c>
-      <c r="M19" s="4">
+      <c r="N19" s="4">
         <v>99.0</v>
-      </c>
-      <c r="N19" s="4">
-        <v>101.0</v>
       </c>
       <c r="O19" s="4">
         <v>101.0</v>
       </c>
       <c r="P19" s="4">
+        <v>101.0</v>
+      </c>
+      <c r="Q19" s="4">
         <v>109.0</v>
       </c>
-      <c r="Q19" s="4">
+      <c r="R19" s="4">
         <v>105.0</v>
       </c>
     </row>
@@ -8501,51 +8583,54 @@
         <v>2025.0</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" s="4">
+        <v>74</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="4">
         <v>113.0</v>
       </c>
-      <c r="E20" s="4">
+      <c r="F20" s="4">
         <v>114.0</v>
       </c>
-      <c r="F20" s="4">
+      <c r="G20" s="4">
         <v>119.0</v>
       </c>
-      <c r="G20" s="4">
+      <c r="H20" s="4">
         <v>108.0</v>
       </c>
-      <c r="H20" s="4">
+      <c r="I20" s="4">
         <v>111.0</v>
       </c>
-      <c r="I20" s="4">
+      <c r="J20" s="4">
         <v>135.0</v>
       </c>
-      <c r="J20" s="4">
+      <c r="K20" s="4">
         <v>107.0</v>
       </c>
-      <c r="K20" s="4">
+      <c r="L20" s="4">
         <v>96.0</v>
       </c>
-      <c r="L20" s="4">
+      <c r="M20" s="4">
         <v>102.0</v>
       </c>
-      <c r="M20" s="4">
+      <c r="N20" s="4">
         <v>107.0</v>
       </c>
-      <c r="N20" s="4">
+      <c r="O20" s="4">
         <v>97.0</v>
       </c>
-      <c r="O20" s="4">
+      <c r="P20" s="4">
         <v>109.0</v>
       </c>
-      <c r="P20" s="4">
+      <c r="Q20" s="4">
         <v>92.0</v>
       </c>
-      <c r="Q20" s="4">
+      <c r="R20" s="4">
         <v>105.0</v>
       </c>
     </row>
@@ -8554,51 +8639,54 @@
         <v>2025.0</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="4">
+        <v>76</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="4">
         <v>101.0</v>
       </c>
-      <c r="E21" s="4">
+      <c r="F21" s="4">
         <v>102.0</v>
       </c>
-      <c r="F21" s="4">
+      <c r="G21" s="4">
         <v>93.0</v>
       </c>
-      <c r="G21" s="4">
+      <c r="H21" s="4">
         <v>102.0</v>
       </c>
-      <c r="H21" s="4">
+      <c r="I21" s="4">
         <v>101.0</v>
       </c>
-      <c r="I21" s="4">
+      <c r="J21" s="4">
         <v>109.0</v>
       </c>
-      <c r="J21" s="4">
+      <c r="K21" s="4">
         <v>97.0</v>
       </c>
-      <c r="K21" s="4">
+      <c r="L21" s="4">
         <v>100.0</v>
-      </c>
-      <c r="L21" s="4">
-        <v>102.0</v>
       </c>
       <c r="M21" s="4">
         <v>102.0</v>
       </c>
       <c r="N21" s="4">
+        <v>102.0</v>
+      </c>
+      <c r="O21" s="4">
         <v>99.0</v>
       </c>
-      <c r="O21" s="4">
+      <c r="P21" s="4">
         <v>101.0</v>
       </c>
-      <c r="P21" s="4">
+      <c r="Q21" s="4">
         <v>97.0</v>
       </c>
-      <c r="Q21" s="4">
+      <c r="R21" s="4">
         <v>100.0</v>
       </c>
     </row>
@@ -8607,51 +8695,54 @@
         <v>2025.0</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" s="4">
+        <v>78</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="4">
         <v>99.0</v>
       </c>
-      <c r="E22" s="4">
+      <c r="F22" s="4">
         <v>100.0</v>
-      </c>
-      <c r="F22" s="4">
-        <v>99.0</v>
       </c>
       <c r="G22" s="4">
         <v>99.0</v>
       </c>
       <c r="H22" s="4">
+        <v>99.0</v>
+      </c>
+      <c r="I22" s="4">
         <v>100.0</v>
       </c>
-      <c r="I22" s="4">
+      <c r="J22" s="4">
         <v>110.0</v>
-      </c>
-      <c r="J22" s="4">
-        <v>102.0</v>
       </c>
       <c r="K22" s="4">
         <v>102.0</v>
       </c>
       <c r="L22" s="4">
+        <v>102.0</v>
+      </c>
+      <c r="M22" s="4">
         <v>100.0</v>
       </c>
-      <c r="M22" s="4">
+      <c r="N22" s="4">
         <v>99.0</v>
       </c>
-      <c r="N22" s="4">
+      <c r="O22" s="4">
         <v>97.0</v>
       </c>
-      <c r="O22" s="4">
+      <c r="P22" s="4">
         <v>101.0</v>
       </c>
-      <c r="P22" s="4">
+      <c r="Q22" s="4">
         <v>99.0</v>
       </c>
-      <c r="Q22" s="4">
+      <c r="R22" s="4">
         <v>100.0</v>
       </c>
     </row>
@@ -8660,51 +8751,54 @@
         <v>2025.0</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" s="4">
+        <v>80</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="4">
         <v>99.0</v>
       </c>
-      <c r="E23" s="4">
+      <c r="F23" s="4">
         <v>98.0</v>
       </c>
-      <c r="F23" s="4">
+      <c r="G23" s="4">
         <v>106.0</v>
       </c>
-      <c r="G23" s="4">
+      <c r="H23" s="4">
         <v>96.0</v>
       </c>
-      <c r="H23" s="4">
+      <c r="I23" s="4">
         <v>98.0</v>
       </c>
-      <c r="I23" s="4">
+      <c r="J23" s="4">
         <v>84.0</v>
       </c>
-      <c r="J23" s="4">
+      <c r="K23" s="4">
         <v>110.0</v>
       </c>
-      <c r="K23" s="4">
+      <c r="L23" s="4">
         <v>100.0</v>
       </c>
-      <c r="L23" s="4">
+      <c r="M23" s="4">
         <v>97.0</v>
       </c>
-      <c r="M23" s="4">
+      <c r="N23" s="4">
         <v>98.0</v>
       </c>
-      <c r="N23" s="4">
+      <c r="O23" s="4">
         <v>101.0</v>
       </c>
-      <c r="O23" s="4">
+      <c r="P23" s="4">
         <v>96.0</v>
       </c>
-      <c r="P23" s="4">
+      <c r="Q23" s="4">
         <v>98.0</v>
       </c>
-      <c r="Q23" s="4">
+      <c r="R23" s="4">
         <v>103.0</v>
       </c>
     </row>
@@ -8713,51 +8807,54 @@
         <v>2025.0</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" s="4">
+        <v>82</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="4">
         <v>99.0</v>
       </c>
-      <c r="E24" s="4">
+      <c r="F24" s="4">
         <v>98.0</v>
-      </c>
-      <c r="F24" s="4">
-        <v>96.0</v>
       </c>
       <c r="G24" s="4">
         <v>96.0</v>
       </c>
       <c r="H24" s="4">
+        <v>96.0</v>
+      </c>
+      <c r="I24" s="4">
         <v>97.0</v>
       </c>
-      <c r="I24" s="4">
+      <c r="J24" s="4">
         <v>105.0</v>
-      </c>
-      <c r="J24" s="4">
-        <v>104.0</v>
       </c>
       <c r="K24" s="4">
         <v>104.0</v>
       </c>
       <c r="L24" s="4">
+        <v>104.0</v>
+      </c>
+      <c r="M24" s="4">
         <v>101.0</v>
       </c>
-      <c r="M24" s="4">
+      <c r="N24" s="4">
         <v>96.0</v>
       </c>
-      <c r="N24" s="4">
+      <c r="O24" s="4">
         <v>103.0</v>
       </c>
-      <c r="O24" s="4">
+      <c r="P24" s="4">
         <v>97.0</v>
       </c>
-      <c r="P24" s="4">
+      <c r="Q24" s="4">
         <v>103.0</v>
       </c>
-      <c r="Q24" s="4">
+      <c r="R24" s="4">
         <v>100.0</v>
       </c>
     </row>
@@ -8766,13 +8863,13 @@
         <v>2025.0</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D25" s="4">
-        <v>100.0</v>
+        <v>84</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="E25" s="4">
         <v>100.0</v>
@@ -8784,33 +8881,36 @@
         <v>100.0</v>
       </c>
       <c r="H25" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="I25" s="4">
         <v>99.0</v>
       </c>
-      <c r="I25" s="4">
+      <c r="J25" s="4">
         <v>96.0</v>
       </c>
-      <c r="J25" s="4">
+      <c r="K25" s="4">
         <v>100.0</v>
-      </c>
-      <c r="K25" s="4">
-        <v>98.0</v>
       </c>
       <c r="L25" s="4">
         <v>98.0</v>
       </c>
       <c r="M25" s="4">
+        <v>98.0</v>
+      </c>
+      <c r="N25" s="4">
         <v>100.0</v>
       </c>
-      <c r="N25" s="4">
+      <c r="O25" s="4">
         <v>102.0</v>
       </c>
-      <c r="O25" s="4">
+      <c r="P25" s="4">
         <v>99.0</v>
       </c>
-      <c r="P25" s="4">
+      <c r="Q25" s="4">
         <v>101.0</v>
       </c>
-      <c r="Q25" s="4">
+      <c r="R25" s="4">
         <v>100.0</v>
       </c>
     </row>
@@ -8819,51 +8919,54 @@
         <v>2025.0</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D26" s="4">
+        <v>86</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="4">
         <v>96.0</v>
       </c>
-      <c r="E26" s="4">
+      <c r="F26" s="4">
         <v>98.0</v>
       </c>
-      <c r="F26" s="4">
+      <c r="G26" s="4">
         <v>100.0</v>
       </c>
-      <c r="G26" s="4">
+      <c r="H26" s="4">
         <v>97.0</v>
       </c>
-      <c r="H26" s="4">
+      <c r="I26" s="4">
         <v>94.0</v>
       </c>
-      <c r="I26" s="4">
+      <c r="J26" s="4">
         <v>87.0</v>
       </c>
-      <c r="J26" s="4">
+      <c r="K26" s="4">
         <v>99.0</v>
       </c>
-      <c r="K26" s="4">
+      <c r="L26" s="4">
         <v>101.0</v>
       </c>
-      <c r="L26" s="4">
+      <c r="M26" s="4">
         <v>102.0</v>
       </c>
-      <c r="M26" s="4">
+      <c r="N26" s="4">
         <v>97.0</v>
       </c>
-      <c r="N26" s="4">
+      <c r="O26" s="4">
         <v>101.0</v>
       </c>
-      <c r="O26" s="4">
+      <c r="P26" s="4">
         <v>96.0</v>
       </c>
-      <c r="P26" s="4">
+      <c r="Q26" s="4">
         <v>110.0</v>
       </c>
-      <c r="Q26" s="4">
+      <c r="R26" s="4">
         <v>99.0</v>
       </c>
     </row>
@@ -8872,51 +8975,54 @@
         <v>2025.0</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D27" s="4">
+        <v>88</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="4">
         <v>101.0</v>
       </c>
-      <c r="E27" s="4">
+      <c r="F27" s="4">
         <v>102.0</v>
       </c>
-      <c r="F27" s="4">
+      <c r="G27" s="4">
         <v>107.0</v>
       </c>
-      <c r="G27" s="4">
+      <c r="H27" s="4">
         <v>99.0</v>
       </c>
-      <c r="H27" s="4">
+      <c r="I27" s="4">
         <v>97.0</v>
       </c>
-      <c r="I27" s="4">
+      <c r="J27" s="4">
         <v>102.0</v>
       </c>
-      <c r="J27" s="4">
+      <c r="K27" s="4">
         <v>105.0</v>
       </c>
-      <c r="K27" s="4">
+      <c r="L27" s="4">
         <v>101.0</v>
       </c>
-      <c r="L27" s="4">
+      <c r="M27" s="4">
         <v>100.0</v>
       </c>
-      <c r="M27" s="4">
+      <c r="N27" s="4">
         <v>99.0</v>
-      </c>
-      <c r="N27" s="4">
-        <v>100.0</v>
       </c>
       <c r="O27" s="4">
         <v>100.0</v>
       </c>
       <c r="P27" s="4">
+        <v>100.0</v>
+      </c>
+      <c r="Q27" s="4">
         <v>104.0</v>
       </c>
-      <c r="Q27" s="4">
+      <c r="R27" s="4">
         <v>102.0</v>
       </c>
     </row>
@@ -8925,51 +9031,54 @@
         <v>2025.0</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" s="4">
-        <v>102.0</v>
+        <v>90</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="E28" s="4">
         <v>102.0</v>
       </c>
       <c r="F28" s="4">
+        <v>102.0</v>
+      </c>
+      <c r="G28" s="4">
         <v>100.0</v>
       </c>
-      <c r="G28" s="4">
+      <c r="H28" s="4">
         <v>103.0</v>
       </c>
-      <c r="H28" s="4">
+      <c r="I28" s="4">
         <v>105.0</v>
       </c>
-      <c r="I28" s="4">
+      <c r="J28" s="4">
         <v>98.0</v>
       </c>
-      <c r="J28" s="4">
+      <c r="K28" s="4">
         <v>93.0</v>
       </c>
-      <c r="K28" s="4">
+      <c r="L28" s="4">
         <v>97.0</v>
-      </c>
-      <c r="L28" s="4">
-        <v>101.0</v>
       </c>
       <c r="M28" s="4">
         <v>101.0</v>
       </c>
       <c r="N28" s="4">
+        <v>101.0</v>
+      </c>
+      <c r="O28" s="4">
         <v>102.0</v>
       </c>
-      <c r="O28" s="4">
+      <c r="P28" s="4">
         <v>103.0</v>
       </c>
-      <c r="P28" s="4">
+      <c r="Q28" s="4">
         <v>97.0</v>
       </c>
-      <c r="Q28" s="4">
+      <c r="R28" s="4">
         <v>100.0</v>
       </c>
     </row>
@@ -8978,51 +9087,54 @@
         <v>2025.0</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" s="4">
+        <v>92</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="4">
         <v>98.0</v>
       </c>
-      <c r="E29" s="4">
+      <c r="F29" s="4">
         <v>99.0</v>
       </c>
-      <c r="F29" s="4">
+      <c r="G29" s="4">
         <v>96.0</v>
       </c>
-      <c r="G29" s="4">
+      <c r="H29" s="4">
         <v>101.0</v>
       </c>
-      <c r="H29" s="4">
+      <c r="I29" s="4">
         <v>99.0</v>
       </c>
-      <c r="I29" s="4">
+      <c r="J29" s="4">
         <v>89.0</v>
       </c>
-      <c r="J29" s="4">
+      <c r="K29" s="4">
         <v>94.0</v>
-      </c>
-      <c r="K29" s="4">
-        <v>97.0</v>
       </c>
       <c r="L29" s="4">
         <v>97.0</v>
       </c>
       <c r="M29" s="4">
-        <v>101.0</v>
+        <v>97.0</v>
       </c>
       <c r="N29" s="4">
         <v>101.0</v>
       </c>
       <c r="O29" s="4">
+        <v>101.0</v>
+      </c>
+      <c r="P29" s="4">
         <v>99.0</v>
       </c>
-      <c r="P29" s="4">
+      <c r="Q29" s="4">
         <v>103.0</v>
       </c>
-      <c r="Q29" s="4">
+      <c r="R29" s="4">
         <v>98.0</v>
       </c>
     </row>
@@ -9031,16 +9143,16 @@
         <v>2025.0</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D30" s="4">
+        <v>94</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="4">
         <v>96.0</v>
-      </c>
-      <c r="E30" s="4">
-        <v>97.0</v>
       </c>
       <c r="F30" s="4">
         <v>97.0</v>
@@ -9049,33 +9161,36 @@
         <v>97.0</v>
       </c>
       <c r="H30" s="4">
+        <v>97.0</v>
+      </c>
+      <c r="I30" s="4">
         <v>95.0</v>
       </c>
-      <c r="I30" s="4">
+      <c r="J30" s="4">
         <v>86.0</v>
       </c>
-      <c r="J30" s="4">
+      <c r="K30" s="4">
         <v>101.0</v>
       </c>
-      <c r="K30" s="4">
+      <c r="L30" s="4">
         <v>102.0</v>
       </c>
-      <c r="L30" s="4">
+      <c r="M30" s="4">
         <v>100.0</v>
       </c>
-      <c r="M30" s="4">
+      <c r="N30" s="4">
         <v>98.0</v>
       </c>
-      <c r="N30" s="4">
+      <c r="O30" s="4">
         <v>102.0</v>
       </c>
-      <c r="O30" s="4">
+      <c r="P30" s="4">
         <v>98.0</v>
       </c>
-      <c r="P30" s="4">
+      <c r="Q30" s="4">
         <v>104.0</v>
       </c>
-      <c r="Q30" s="4">
+      <c r="R30" s="4">
         <v>99.0</v>
       </c>
     </row>
@@ -9084,51 +9199,54 @@
         <v>2025.0</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D31" s="4">
+        <v>96</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="4">
         <v>97.0</v>
       </c>
-      <c r="E31" s="4">
+      <c r="F31" s="4">
         <v>96.0</v>
       </c>
-      <c r="F31" s="4">
+      <c r="G31" s="4">
         <v>99.0</v>
-      </c>
-      <c r="G31" s="4">
-        <v>102.0</v>
       </c>
       <c r="H31" s="4">
         <v>102.0</v>
       </c>
       <c r="I31" s="4">
+        <v>102.0</v>
+      </c>
+      <c r="J31" s="4">
         <v>110.0</v>
       </c>
-      <c r="J31" s="4">
+      <c r="K31" s="4">
         <v>91.0</v>
       </c>
-      <c r="K31" s="4">
+      <c r="L31" s="4">
         <v>98.0</v>
       </c>
-      <c r="L31" s="4">
+      <c r="M31" s="4">
         <v>97.0</v>
       </c>
-      <c r="M31" s="4">
+      <c r="N31" s="4">
         <v>104.0</v>
       </c>
-      <c r="N31" s="4">
+      <c r="O31" s="4">
         <v>97.0</v>
       </c>
-      <c r="O31" s="4">
+      <c r="P31" s="4">
         <v>98.0</v>
       </c>
-      <c r="P31" s="4">
+      <c r="Q31" s="4">
         <v>94.0</v>
       </c>
-      <c r="Q31" s="4">
+      <c r="R31" s="4">
         <v>96.0</v>
       </c>
     </row>
@@ -9152,31 +9270,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2">
@@ -9184,7 +9302,7 @@
         <v>2025.0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4">
         <v>99.0</v>
@@ -9216,7 +9334,7 @@
         <v>2025.0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C3" s="4">
         <v>103.0</v>
@@ -9248,7 +9366,7 @@
         <v>2025.0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C4" s="4">
         <v>104.0</v>
@@ -9280,7 +9398,7 @@
         <v>2025.0</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4">
         <v>100.0</v>
@@ -9312,7 +9430,7 @@
         <v>2025.0</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C6" s="4">
         <v>100.0</v>
@@ -9344,7 +9462,7 @@
         <v>2025.0</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C7" s="4">
         <v>101.0</v>
@@ -9376,7 +9494,7 @@
         <v>2025.0</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C8" s="4">
         <v>103.0</v>
@@ -9408,7 +9526,7 @@
         <v>2025.0</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C9" s="4">
         <v>101.0</v>
@@ -9440,7 +9558,7 @@
         <v>2025.0</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C10" s="4">
         <v>97.0</v>
@@ -9472,7 +9590,7 @@
         <v>2025.0</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C11" s="4">
         <v>100.0</v>
@@ -9504,7 +9622,7 @@
         <v>2025.0</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C12" s="4">
         <v>95.0</v>
@@ -9536,7 +9654,7 @@
         <v>2025.0</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C13" s="4">
         <v>100.0</v>
@@ -9568,7 +9686,7 @@
         <v>2025.0</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C14" s="4">
         <v>99.0</v>
@@ -9600,7 +9718,7 @@
         <v>2025.0</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C15" s="4">
         <v>97.0</v>
@@ -9632,7 +9750,7 @@
         <v>2025.0</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C16" s="4">
         <v>102.0</v>
@@ -9664,7 +9782,7 @@
         <v>2025.0</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C17" s="4">
         <v>102.0</v>
@@ -9696,7 +9814,7 @@
         <v>2025.0</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C18" s="4">
         <v>102.0</v>
@@ -9728,7 +9846,7 @@
         <v>2025.0</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C19" s="4">
         <v>101.0</v>
@@ -9760,7 +9878,7 @@
         <v>2025.0</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C20" s="4">
         <v>108.0</v>
@@ -9792,7 +9910,7 @@
         <v>2025.0</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C21" s="4">
         <v>102.0</v>
@@ -9824,7 +9942,7 @@
         <v>2025.0</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C22" s="4">
         <v>101.0</v>
@@ -9856,7 +9974,7 @@
         <v>2025.0</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C23" s="4">
         <v>98.0</v>
@@ -9888,7 +10006,7 @@
         <v>2025.0</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C24" s="4">
         <v>94.0</v>
@@ -9920,7 +10038,7 @@
         <v>2025.0</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C25" s="4">
         <v>103.0</v>
@@ -9952,7 +10070,7 @@
         <v>2025.0</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C26" s="4">
         <v>98.0</v>
@@ -9984,7 +10102,7 @@
         <v>2025.0</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C27" s="4">
         <v>100.0</v>
@@ -10016,7 +10134,7 @@
         <v>2025.0</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C28" s="4">
         <v>102.0</v>
@@ -10048,7 +10166,7 @@
         <v>2025.0</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C29" s="4">
         <v>100.0</v>
@@ -10080,7 +10198,7 @@
         <v>2025.0</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C30" s="4">
         <v>97.0</v>
@@ -10112,7 +10230,7 @@
         <v>2025.0</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C31" s="4">
         <v>100.0</v>

</xml_diff>